<commit_message>
Updated for open house/presentations/filming
</commit_message>
<xml_diff>
--- a/weeks/PresentationScheduleAsOf2017-04-04.xlsx
+++ b/weeks/PresentationScheduleAsOf2017-04-04.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Presentations</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>Industry</t>
+  </si>
+  <si>
+    <t>Farmbot</t>
+  </si>
+  <si>
+    <t>AutoVehicle</t>
+  </si>
+  <si>
+    <t>SmartHive</t>
+  </si>
+  <si>
+    <t>LabFlow - Presenting on Tuesday instead of Saturday</t>
+  </si>
+  <si>
+    <t>Solar</t>
   </si>
 </sst>
 </file>
@@ -390,7 +405,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,6 +568,9 @@
         <f t="shared" ref="B15:B23" si="1">B14+TIME(0,15,0)</f>
         <v>0.57291666666666663</v>
       </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -563,6 +581,9 @@
         <f t="shared" si="1"/>
         <v>0.58333333333333326</v>
       </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -572,6 +593,9 @@
         <f t="shared" si="1"/>
         <v>0.59374999999999989</v>
       </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -582,6 +606,9 @@
         <f t="shared" si="1"/>
         <v>0.60416666666666652</v>
       </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -590,6 +617,9 @@
       <c r="B19" s="1">
         <f t="shared" si="1"/>
         <v>0.61458333333333315</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ambient moved an hour earlier
</commit_message>
<xml_diff>
--- a/weeks/PresentationScheduleAsOf2017-04-04.xlsx
+++ b/weeks/PresentationScheduleAsOf2017-04-04.xlsx
@@ -405,7 +405,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +446,7 @@
         <v>0.38541666666666669</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -458,7 +458,7 @@
         <v>0.39583333333333337</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -470,7 +470,7 @@
         <v>0.40625000000000006</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -482,7 +482,7 @@
         <v>0.41666666666666674</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -494,7 +494,7 @@
         <v>0.42708333333333343</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>